<commit_message>
added graphs for some correlations, cleaned up dataframe
</commit_message>
<xml_diff>
--- a/AnnualLobyingOnDairy.xlsx
+++ b/AnnualLobyingOnDairy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Floor Kouwenberg\Documents\VU\Data Wrangling\Data-Wrangling-Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laniepreston/Documents/Data_Wrangling/Data-Wrangling-Final-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A42A9B29-73E2-448F-AD23-768B189D42D8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EBFD8F-A479-864C-ACA9-CEDB89A7FC56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11148" yWindow="2868" windowWidth="17280" windowHeight="8964"/>
+    <workbookView xWindow="11060" yWindow="2540" windowWidth="17280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="{worksheet}" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Dollar</t>
+    <t>Total Lobbies</t>
+  </si>
+  <si>
+    <t>Lobbies to Democrats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lobbies to Republicans </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -509,7 +515,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -517,6 +523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -543,24 +550,24 @@
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Berekening" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Controlecel" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Gekoppelde cel" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Goed" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Invoer" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Kop 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Kop 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Kop 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Kop 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutraal" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notitie" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ongeldig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Totaal" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uitvoer" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -576,7 +583,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -871,36 +878,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G24" sqref="G23:G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1998</v>
       </c>
       <c r="B2" s="2">
         <v>2245000</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>707800</v>
+      </c>
+      <c r="D2">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1999</v>
       </c>
@@ -908,15 +927,21 @@
         <v>3051110</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2000</v>
       </c>
       <c r="B4" s="2">
         <v>2798900</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>809200</v>
+      </c>
+      <c r="D4">
+        <v>2100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2001</v>
       </c>
@@ -924,15 +949,21 @@
         <v>3260000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2002</v>
       </c>
       <c r="B6" s="2">
         <v>4314700</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>918200</v>
+      </c>
+      <c r="D6">
+        <v>2200000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2003</v>
       </c>
@@ -940,15 +971,21 @@
         <v>4073436</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2004</v>
       </c>
       <c r="B8" s="2">
         <v>4839800</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>1000000</v>
+      </c>
+      <c r="D8">
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2005</v>
       </c>
@@ -956,15 +993,21 @@
         <v>4841312</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2006</v>
       </c>
       <c r="B10" s="2">
         <v>3840045</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>1100000</v>
+      </c>
+      <c r="D10">
+        <v>2900000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2007</v>
       </c>
@@ -972,15 +1015,21 @@
         <v>5220448</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2008</v>
       </c>
       <c r="B12" s="2">
         <v>4853491</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>2000000</v>
+      </c>
+      <c r="D12">
+        <v>3100000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2009</v>
       </c>
@@ -988,15 +1037,21 @@
         <v>4832390</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2010</v>
       </c>
       <c r="B14" s="2">
         <v>5662885</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>1600000</v>
+      </c>
+      <c r="D14">
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>2011</v>
       </c>
@@ -1004,15 +1059,21 @@
         <v>6695032</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2012</v>
       </c>
       <c r="B16" s="2">
         <v>7302248</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>999000</v>
+      </c>
+      <c r="D16">
+        <v>3700000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2013</v>
       </c>
@@ -1020,15 +1081,21 @@
         <v>8347149</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2014</v>
       </c>
       <c r="B18" s="2">
         <v>6951794</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>791500</v>
+      </c>
+      <c r="D18">
+        <v>2800000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2015</v>
       </c>
@@ -1036,15 +1103,21 @@
         <v>7116441</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>2016</v>
       </c>
       <c r="B20" s="2">
         <v>6480567</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>943400</v>
+      </c>
+      <c r="D20">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2017</v>
       </c>
@@ -1052,15 +1125,21 @@
         <v>6009870</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>2018</v>
       </c>
       <c r="B22" s="2">
         <v>7590843</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>821200</v>
+      </c>
+      <c r="D22">
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>2019</v>
       </c>

</xml_diff>